<commit_message>
cambio columnas excel google
</commit_message>
<xml_diff>
--- a/admin-tao-master/template_google.xlsx
+++ b/admin-tao-master/template_google.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taois\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\neumatruck\admin-tao-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C498B7D8-9468-4129-B261-DFF6447EEDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ECC92A-A5BA-4A29-A0C9-95A50087B428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="1980" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,6 @@
     <t>descripción</t>
   </si>
   <si>
-    <t>enlace al producto</t>
-  </si>
-  <si>
-    <t>estado (nuevo)</t>
-  </si>
-  <si>
     <t>precio</t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>categoría en google product</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>estado</t>
   </si>
 </sst>
 </file>
@@ -138,14 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,7 +366,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -380,44 +379,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>